<commit_message>
Get daily reddit data: Tue Oct 22 08:10:53 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_27.xlsx
+++ b/data/collected_data/2024_10_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3135 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1g9bzw5</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Shimmery pink with soft gold chrome</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9bzw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1g98vma</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Gel nails I did on myself-
+"Latte" themed :) Inspired by Japanese nail art I see a lot on instagram!</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g98vma</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1g999se</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Inspired by my garden grown beans. And I used a loofah gourd for the pattern!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g999se</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1g98n6e</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beauty is pain </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g98n6e/beauty_is_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1g986eb</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Am I being over critical or are these nails a mess?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g986eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1g96odq</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Chocolate Gold 🤎⚜️ #cateyenails #3dnails #fallnails #nailart #chrome #go...</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/h4Ny7c2pS6w?feature=shared</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1g96m1l</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Ex nail biter- proud progress :D</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g96m1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1g94rgv</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>HELP builder gel</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g94rgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1g94mma</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">That cat that inspired the nail art🐈‍⬛💗 press ons, hand painted by me @arisnailartistry on instagram </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g94mma</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1g9bokq</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Iridescent peacock nails, I can’t stop looking at them </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i979jg1p49wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1g9bm2t</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Someone did my acrylics and my pinkie looks funny.</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi63hmyr39wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1g9av4w</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Growing out bitten nails- looking for advice </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9av4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1g9a5v1</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>In love with the holo 💿</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9a5v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1g9a4so</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My pink halloween nails!! 💅😍🎃🕸🕷</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9a4so</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1g9a3x8</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>got my nails done professionally for the first time in three years 💕</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/577z78zyl8wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1g99gda</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>My second ever pedicure and she did such a great job! So pretty 💙</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ygw53gze8wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1g987ll</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Boys and girls of every age, wouldn’t you like to see something strange?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qolv1zgx28wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1g986bd</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>These are bad, right?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g986bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1g983ya</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Painted my nails for Halloween, I couldn’t get the nail polish off my skin. Opinions on them?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3380fity18wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1g9810o</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Proud of how long they’ve grown without breaking </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9810o</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1g980ck</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Halloween Gel-X set I did myself!</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://imgur.com/KpUmTng</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1g97v4s</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Spoopy Combo 🧟‍♂️</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g97v4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1g97k7e</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>textured polish part 2 - road stripe nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rph2tzltw7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1g97j2t</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>thoughts on this set?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g97j2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1g979zn</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Fall Nails 🤎</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g979zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1g97770</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>You guys 😫</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz3qrv2lt7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1g96xsh</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suggestions for quality top coat gel and UV light. </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g96xsh/suggestions_for_quality_top_coat_gel_and_uv_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1g96qfb</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Clear structured gel?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g96qfb/clear_structured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1g966e8</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Can I use a bandaid to protect my nail from cracking further for now? (sensory issue of short nails)</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zm0dap9k7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1g95lzb</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween treats 👻 </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g95lzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1g95ixr</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted my nails and I love them :) I’m so happy </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnxfcenie7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1g957ze</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>purple press-ons 💜🍂</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzjr5k37c7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1g957bb</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My spooky nails 👻</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7syob72c7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1g9500o</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green Chrome Frenchie </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9500o</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1g94tuv</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>First time nail appointment advice</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g94tuv/first_time_nail_appointment_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1g94ymk</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Seche Vite QDTC: user error??</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g94ymk/seche_vite_qdtc_user_error/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1g94ou5</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Doesn’t look like much but this is a career high for me- the hard gel baby boomer </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s01ca4pj77wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1g94cm6</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Fresh Set 💅🏾</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c4yi3ul47wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1g93vfm</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Black and white lovers</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1t482yj07wd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1g939uy</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Saw inspired nails 💉💉</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh2uj6mkv6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1g93mw7</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>simple, but love this color</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mhaps8hy6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1g93dte</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moms mani ! </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8px8hihw6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1g92ugr</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Ignore the bad gel work 🥲 I'm still learning. But this is my first time doing nail art. 🤣</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aokt8zxzr6wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1g92lf4</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Wednesday nails</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk2nyl0zp6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1g924n4</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Cracked thumb nail</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f03bawqdm6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1g9248z</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>think i’m becoming an almond girlieee🫢</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9248z</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1g91vgk</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Spooky set 👻</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcuku71fk6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1g90twe</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>BuilderGel only lasts 48 hours, Help!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g90twe/buildergel_only_lasts_48_hours_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1g91iyz</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Just tried Gel-X on myself for the first time!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g91iyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1g91i3v</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not the color I chose but ended up even better </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i05c3hgkh6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1g91c6d</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce Peek a Boo Halloween nails </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g91c6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1g914fk</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Dilemma </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g914fk/nail_dilemma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1g90o3h</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My wedding nails, done by me</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g90o3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1g90m85</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Pumpkin nail set 🥰💞🎃</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msp9hupya6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1g90dut</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nail care help.</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g90dut/nail_care_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1g90bu6</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>My newest set. Loving them something wicked! 🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x17um0pu86wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1g8znv6</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>I can’t stop seeing my beautiful new nails 😍 a little mixed with Halloween, don’t you think?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tjciz1346wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1g8z8a2</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Leave it or add stuff?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edas6u2116wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1g8ysio</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>autumn colours by Lewes Nails 🍁🍂🎃</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jamq72uxx5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1g8ylmz</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Simple, yet spooky</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02r4bk0kw5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1g8ygcd</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grow out appreciation! </t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8sbiyggv5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1g8ydra</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Boyfriend broke up with me but at least now I get to have pretty nails again</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r229b7jxu5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1g8y2bu</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Second DIY set ever</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bpsxqons5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1g8xpnv</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Temporarily painting over nails?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8xpnv/temporarily_painting_over_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1g8xamr</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">any tips to stop biting the skin around my nails? I’ve been growing my nails out and being kind to them, so it’s like grrrr :( </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8xamr/any_tips_to_stop_biting_the_skin_around_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1g8x9hs</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🎃 🕷️ 🕸️ </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8x9hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1g8x4qw</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I being unreasonable? Looking for advice on a nail salon experience. </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8x4qw/am_i_being_unreasonable_looking_for_advice_on_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1g8vouw</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Consistent Break Point</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7gcwfenb5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1g8wy1j</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Can I use regular nail polish on nail tips?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8wy1j/can_i_use_regular_nail_polish_on_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1g8wxjl</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumnal chrome </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52o0aujjk5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1g8wp51</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Black and silver nails</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka53derui5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1g8wjns</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>What are we calling these…</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8wjns</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1g8wcp0</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween set </t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8wcp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1g8w9dw</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need advice! </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8w9dw/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1g8vdii</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Witch please 🔮</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb86eule95wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1g8unc2</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Smoky tip</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qel29ff745wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1g8uiro</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>it's the most fabulous time of the year</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8uiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1g8u8qr</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried a new shape </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8ezboeb15wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1g8u2x7</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Cuticle work</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8u2x7</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1g8txvi</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Wedding nails!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7vg28v5z4wd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1g8twgl</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Gel red nails on my own nails❤️</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtlu4luvy4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1g8tbbt</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some Recent Nails </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8tbbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1g8t6a3</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Need advice, please!</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8t6a3/need_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1g8t2mv</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Spooky nails 👻</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc4mzkdys4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1g8sufx</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic nails for the week </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zezyzatcr4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1g8ssii</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark Purple for October/Halloween </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06t1qxmyq4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1g8sqia</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When do you stop painting your toenails? </t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g8sqia/when_do_you_stop_painting_your_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1g8rm4l</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Can I cut my nails down?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywv8pjpai4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1g8ksgg</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>How do you feel about press-ons?? Ishould’ve tried them sooner!!!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6xzcj14l2wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1g8n12u</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Are my natural nails too short?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pkavaned3wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1g8nwjv</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find a sheer jelly pink dupe please! </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yabbos8tm3wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1g8oxy0</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>My first attempt at my own acrylics 🎃</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mloa089iw3wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1g8jm39</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Did my halloween nails a little early</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rglzr53k42wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1g8sg28</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>This color represents me✨😌</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoiu7l5fo4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1g8r8qy</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite sets till date! </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8r8qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1g8qwb1</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Can’t stop looking at my nails after a refresh!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8qwb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1g8qn2i</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>🐁🐀</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l8na5ema4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1g8qefb</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>I always go back to the classic red.</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/708h9t5r84wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1g8q3n8</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Nails made by my MIL😅</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2v8u06c64wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1g8phrg</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Since you loved my current set. Here was early October 🕸️</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpynp0z714wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1g9cev7</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>ILNP - UK?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9cev7/ilnp_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1g9c6dp</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Dupe Alert: Dam La Tour Eiffel and Zoya Patrice</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9c6dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1g9b5eo</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Repair Mode </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbfn8rq9y8wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1g9amzr</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Perfect brown shade</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo4f9l7yr8wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1g9a76g</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail bed burns </t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9a76g/nail_bed_burns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1g9a6gz</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I see we've been posting flakies in jelly </t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6wl0s2hqm8wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1g98b56</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>What nail shape should I go for?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g98b56</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1g97y7p</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Spoopy Combo 🧟‍♂️</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g97y7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1g97i4z</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Wishful Thinking 🧲</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/amxrvixaw7wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1g96vry</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Application, 2 days apart </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g96vry</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1g96vds</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>I’m ready for Halloween</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8m7azvgoq7wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1g961zf</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Wdyt of this minihaul from Starrily? Should I rather go with a different brand for these/similar polishes?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxxbtoosi7wd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1g95sj1</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Can't stand long nails, can I still paint my nails?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g95sj1/cant_stand_long_nails_can_i_still_paint_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1g95pu3</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>this post is solely about my nail polish and is in no way me showing off the current state of my cuticles</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsx968j1g7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1g953z8</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips on how to care for my nails? </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p89w5y7b7wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1g93z3i</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Shifty blue magic🦋☔️</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g93z3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1g93b86</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soooo sparkly! </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/khsorgjuv6wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1g939x0</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>First try at stamping, first mani showoff</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g939x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1g9343a</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail polish do you get the most compliments on? </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9343a/what_nail_polish_do_you_get_the_most_compliments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1g92vi8</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>By Dany Vianna Brinde 🎃✨</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g92vi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1g92txx</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Magical 🪄🧙</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g92txx</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1g92a0y</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Y’all, deep space is something else</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g92a0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1g91pg6</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simply Eerie-sistable </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g91pg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1g91i4o</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Essie Fairy Tailor doesn't dry hard?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g91i4o/essie_fairy_tailor_doesnt_dry_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1g91dzn</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Went in too hard with the e-file around my cuticles and ended up filing down the nail plate excessively— how do I fix this?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g91dzn/went_in_too_hard_with_the_efile_around_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1g91aj1</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce Peek a Boo Halloween nails </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g91aj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1g9185j</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>blue memorial flower art</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9185j</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1g90w8e</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Nail design on Xray</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy7elrujb4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1g90j3x</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>it finally happened to me :(</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g90j3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1g8zrxc</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Light My Fire🔥</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj5i1rov46wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1g8z6qr</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New fav thermal alert </t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8z6qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1g8z1sc</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m not crazy you’re crazy </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0ula4qrz5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1g8ye0u</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Favorite LynBDesigns polishes?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8ye0u/favorite_lynbdesigns_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1g8xkh8</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Loving this Halloween set I did 🥹</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8xkh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1g8x6mm</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>No Illusions from KBShimmer has me staring at my nails all dang day</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8x6mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1g8x5ho</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncats Boa Constrictor 🐍 </t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8x5ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1g8wozy</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>First Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8wozy/first_lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1g8wlnd</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>BAT! 🦇</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8wlnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1g8wgt2</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> you had me at halo </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8wgt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1g8w6ou</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal Vampyr mystery polish </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8w6ou</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1g8vuem</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Glow in the dark stamping polish?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8vuem/glow_in_the_dark_stamping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1g8vs5k</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at gel </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8vs5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1g8vqch</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Didn’t plan to match my sweatshirt </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q7wibvxb5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1g8voyy</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>🫧</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8voyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1g8vh5q</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Please help me save this nail!!!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8vh5q/please_help_me_save_this_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1g8vfmz</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>The gloomier the weather, the brighter my nails will be</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8vfmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1g8v568</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>This red makes me ready for the holidays already!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3npga68r75wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1g8uksg</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Team candy corn 🍬🌽</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8uksg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1g8tjhb</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Nail polish for tv appearance?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8tjhb/nail_polish_for_tv_appearance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1g8t8e2</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>My third pair of halloween nails 🖤🔪</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8t8e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1g8spe9</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Help ID this OPI shade</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8spe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1g8s896</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>my 30th birthday mani. ✨💕🎂</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8s896</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1g8s47u</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>I've been looking for magnetic nail polish everywhere! Please help!</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8s47u/ive_been_looking_for_magnetic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1g8rxxf</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Summerween!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrl3qxbpk4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1g8rrr7</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations for stamping tutorials </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8rrr7/recommendations_for_stamping_tutorials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1g8rk0q</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>We Are The Ones Who Dwell Within</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8rk0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1g8qv70</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For Ghibli fans: super easy soot sprite nails for Halloween! </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqwoo92fc4wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1g8qs9t</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Is this shrinkage or just from application?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8qs9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1g8pqe2</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wow! I guess I'm a flakie girly now </t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8pqe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1g8piqv</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>I'm SH00K</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8piqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1g8paqs</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Just simple pastels 😁</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i86s5mwjz3wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1g8oc05</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Halloween thermal nail art 🕸🎃</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8oc05</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1g8hh1g</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>obsessed with the flakes 💜(mooncat forces of evil)</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8hh1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1g8myoy</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Spooky little aliens are abducting my attention 👽🛸</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8myoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1g8m1jk</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g8m1jk/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1g9d0h3</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Does anyone else LOVE big gemstones/charms?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g9d0h3/does_anyone_else_love_big_gemstonescharms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1g9af07</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Halloween Party Nails!!!🎃🎉</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/43wet2vbp8wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1g95mpd</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween treats 👻 </t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g95mpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1g94l58</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The cat that inspired the nail art 🐈‍⬛💗 press ons hand painted by me @arisnailartistry on instagram </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g94l58</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1g93ky0</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nightmare Before Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihph3vi2y6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1g934gz</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>tried to make them vampire-esque🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g934gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1g92au9</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They are definitely perfect </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z0nomkfln6wd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1g926d6</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Did these on myself, thoughts?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g926d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1g91wrl</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this effect </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f41y2ypok6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1g90n0r</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Pumpkin nail set 🥰💞🎃 with the cutest tiniest pumpkin I could find</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fac54eq4b6wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1g8zzvo</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Pokemon Nails, gotta catch 'em all!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4w2s07h66wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1g8xncu</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>amateur nail gel-x nail artists in the US: what nail supplies do you wish you could buy in person? and if you already do, where do you go?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g8xncu/amateur_nail_gelx_nail_artists_in_the_us_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1g8waxu</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky but classy </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8waxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1g8w117</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Halloween III Season of the Witch nails!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8w117</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1g8vxo1</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>my design for this month</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gl5c1lvdd5wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1g8vcgd</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Spooky season is amongst us 🔮</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avfpgqm695wd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1g8ueaz</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Practice</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g8ueaz/practice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1g8tg0h</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">aura nails advice </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g8tg0h/aura_nails_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1g8ln8i</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Handpainted classic Art Nails </t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g8ln8i</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Oct 23 08:10:43 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_27.xlsx
+++ b/data/collected_data/2024_10_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C485"/>
+  <dimension ref="A1:C673"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8679,6 +8679,3202 @@
         </is>
       </c>
     </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1ga4qox</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>My friend say my new nails look like cockroaches.........ahhhhhh</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga4qox</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ga4oji</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>My little nails</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga4oji</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ga4g59</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Idk how to take care of my nails! </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga4g59</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ga4aq7</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>cant go wrong with pink 😘</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2i976wvegwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1g9xo12</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Clubbed thumbs Hellppp</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hviwoj8uiewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ga0bzq</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Question!! Does anyone know both the brands Le chat- perfect match and OPI? Do you prefer one over the other? I’m so indecisive!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga0bzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ga2xiq</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>ren faire claws</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga2xiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ga3kq5</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Using regular polish with builder &amp; gel?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ga3kq5/using_regular_polish_with_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ga2zfo</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>october sets</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga2zfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ga2h9m</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Different angle, still love the colour, any tips?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga2h9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ga1vgh</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daphne Blake Nails </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ga1vgh/daphne_blake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ga1lrx</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>🦇🎃Fresh new set as of today. Halloween themed nails! 🦇🎃</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga1lrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ga18mt</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My natural nails</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbl5h8rxffwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1ga0xbv</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Good keyboard covers for long nails?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ga0xbv/good_keyboard_covers_for_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ga0tet</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed 💜🖤 </t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jt7ca11obfwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ga0pm8</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>🩷🩷</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhtxil0pafwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1ga03k0</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Nails </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/niod5hor4fwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1g9zvcm</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Week 2 of Spooky Season</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9zvcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1g9zsqt</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Which color/set</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9zsqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1g9zpeb</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Nail color ideas</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9zpeb/nail_color_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1g9zp2v</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner ◡̈ </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9zp2v/beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1g9zgk0</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday/Halloween nails </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9zgk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1g9z4cv</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Red nails for fall❤️</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9z4cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1g9ye07</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this color for easy everyday manicure </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9cu1kw4pewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1g9ybg3</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Would it be safe to put press ons on my nails while theyre healing after removing gel extensions?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9ybg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1g9xx39</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Crappy Little Nail Art</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9xx39</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1g9xq5z</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was I overcharged? </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agbd84hcjewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1g9xo1v</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like using lots of colors, good or bad mix on this one? </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9xo1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1g9wtnp</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>fall nails!!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvyvgnpkbewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1g9wdpk</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More Fall nails </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a1giqpp7ewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1g9vo8r</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been getting bad manicures in Seattle; thin brittle nails now that are breaking. Any recs ? </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9vo8r/ive_been_getting_bad_manicures_in_seattle_thin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1g9vmb9</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn ready! </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h46o0mze1ewd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1g9vfzv</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Just wanted to show off my new set</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78szspozzdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1g9vfxo</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can't get nails to stay on. </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9vfxo/cant_get_nails_to_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1g9veik</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Baldur’s Gate 3 Nails! What should I make next?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9veik</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1g9v69m</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Nail shape help</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvobvdzmxdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1g9sh82</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how do i keep the nails from falling off in the lamp </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9sh82/how_do_i_keep_the_nails_from_falling_off_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1g9ugyq</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do you like this color??? </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf7xdxp0sdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1g9uf2z</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Progress pics </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9uf2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1g9u9gd</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>my new set</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8gc6jmqcqdwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1g9t2l6</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Scream Nails</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyeo4z99hdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1g9svhw</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Liquid Gold</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy209c3tfdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1g9snju</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Trying to hold on to summer 🍓</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/he6pkvz4edwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1g9slau</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Which nail shape would look best on my hand shape? I feel like I have really manly hands. Any/all advice appreciated.</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4ga211oddwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1g9se6i</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>I liked the color</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo2fuqd2cdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1g9s96v</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9s96v</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1g9s41i</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Nail care help needed!</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p40qcex1adwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1g9s2yp</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>My nail tech killed my vacation nails 🏔️</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9s2yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1g9rp30</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Love 🤎</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmi5zyky6dwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1g9rooj</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Looking for a tutorial to do Zombie Nails myself</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6oikvqt6dwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1g9ri8m</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu3wsnkp5dwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1g9rg6f</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caj6577a5dwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1g9r8lu</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>I choose mat colour but if choice would be yours, what would you pick?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxj8va2r3dwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1g9r5ou</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I crazy? Or do they look kind of weird? </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9r5ou</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1g9qy7g</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">update </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9qy7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1g9qtf6</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Mi trabajo</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5pjoall0dwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1g9p8du</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Dealers Choice Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fw6g7oj2pcwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1g9qgnp</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>What can I do to make my hands look more feminine?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9qgnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1g9q92q</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail care </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkb4izrfwcwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1g9q3dd</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Feel like I finally found my perfect winter nude. I’m a bright winter</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz23ng4bvcwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1g9q2qe</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done for the first time in two years! </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9q2qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1g9q2gw</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Spooky Season Set</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pyu2255vcwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1g9pl7s</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">On the natural nail journey </t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9pl7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1g9osot</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Thoughts on this color?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9osot</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1g9o8ly</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Wanting to get overlays, any advice to care for my natural nails first?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9o8ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1g9mu82</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>embarrassing questionnn</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9mu82/embarrassing_questionnn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1g9n36z</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Builder Gel</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9n36z/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1g9n1qy</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic natural nails </t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhnr6wj29cwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1g9mykh</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Clionadh - Hazard</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9mykh</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1g9mijw</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Luminary vs Dip</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9mijw/luminary_vs_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1g9m6k3</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Halloween set</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9m6k3</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1g9m2tq</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>New to getting my nails done and using a new tech....does this look ok?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9m2tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1g9m1rt</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Only second coat peeled off. Why? </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ko9pspp1cwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1g9lriz</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really like the colour but don't think Kevin is too bothered </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9lriz</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1g9lq87</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need serious help after acrylic nails removal. What do you recommand? </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kp5dqv7zbwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1g9l5mr</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>First time doing cat eye!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss78a8a5vbwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1g9klwn</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween is coming </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ro1pgvs0rbwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1g9k2p7</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I switched up my nails this time.. I get an ombré French with chrome A LOT. I am super indecisive and it never gets old to me. I love it… but I’m starting to really switch them up and I love it!! What do we think? Do we love them, hate them, or are they just okay…</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9k2p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1g9jxag</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second time </t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn6qrhkxlbwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1g9f80c</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Painted my own nude nails</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdlif0hqfawd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1g9jkdq</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Spooky szn nails 👻🦇💜</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9jkdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1g9gffa</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Tools for a buffed manicure?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9gffa/tools_for_a_buffed_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1g9ipyq</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>help decide</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9ipyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1g9iagi</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>CAT URINE SMELL-MMA ?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9iagi/cat_urine_smellmma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1g9guyp</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The holy grail for peeling nails! </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g9guyp/the_holy_grail_for_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1g9j8j1</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>What is the best shape for my nails?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9j8j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1g9hu89</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails 💅🏾 </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9hu89</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1g9fsr2</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got this set for the Release of BEETLEJUICE BEETLEJUICE </t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9fsr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1g9fskg</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Fall nails!🍁🍂✨️</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9fskg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1g9f3zb</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Went on a date and guy had both a cat and a dog. Held both my hands till the last minute 😌</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9f3zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1g9emj6</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Wanted something Halloween themed but still somewhat classy. It's all hand painted by my amazing nail tech, no stickers</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lbp1toh8awd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1g9ejjh</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magical </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkfv5fkj7awd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1g9e2p5</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how do u care for ur nails after getting a set removed? </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8i2orjb1awd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1g9e1qr</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Gone a little out of my comfort zone with this green.. normally a nude gal 😅</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukxu98zx0awd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1g9e1ek</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Simple pink coffin nails 🩷</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9e1ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1g9dgtd</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>spooky diy set 🎃</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9dgtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1ga4eyb</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>pink make em wink x</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1ivgvrdggwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ga2rcl</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>My new job doesn't allow painted nails (working with food) so I'm going to try my hand at something like these to get by!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f13a73p6wfwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ga2hxm</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Playgirl 'Anna'</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/22-10-2024-ri3jesQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ga25az</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Looking for a polish like Bee’s Knee’s Dancing Queens</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ga25az/looking_for_a_polish_like_bees_knees_dancing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1ga1n83</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Talk To Me</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga1n83</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ga15py</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regret adding the green two weeks later! </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2oq522dvefwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ga1217</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Help! My dip keeps peeling</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ga1217/help_my_dip_keeps_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ga0xkl</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>starry night</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8s2aauscfwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ga0332</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a color dupe  </t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywtoki4n4fwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1g9zjqa</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Tips for magnetized polish?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybq4bkpkzewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1g9ygx3</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Orange Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay18f3zspewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1g9ycip</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Birthstones!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdjgo23roewd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1g9xt2p</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Never will I ever have another plain mani</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9xt2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1g9xn68</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Spooky baby, spooky nails.</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9xn68</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1g9xl7m</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Polish - Per Se (thermal)</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vd4otqf3iewd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1g9wid3</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Zoya 'Cynthia '</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx1ero4t8ewd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1g9wfnj</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>White Opal nails using 2 polishes 🤍</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9wfnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1g9wefy</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9wefy</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1g9wbr5</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I never expected my first LynB to be so gorgeous! Clean classic mani with a twist. The orange/pink shimmer makes this a subtle stunner 🤩</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9wbr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1g9w0cd</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Tried something new, cute 🐍 nails</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9w0cd</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1g9vrsc</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Devourer of Souls!!!! </t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9vrsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1g9v8bf</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classy Pumpkin 🎃 </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9v8bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1g9uni2</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted to show off this stunner, Sassy Sauce - Overdrive </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9uni2</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1g9u9ge</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Anybody else's Holo Taco peelie bag falling apart? :(</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9u9ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1g9tz18</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Cuticle butter recs</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9tz18/cuticle_butter_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1g9t53f</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Cock a Doodle Doom in golden hour sunlight 🐓☄️</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8y9uxetohdwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1g9so9e</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of One True Love by Bee's Knees</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9so9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1g9rkal</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed is an understatement - big win for the Orly Color Pass in my book </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huvp7ng16dwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1g9rf7o</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>That purple shimmer tho</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9rf7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1g9r73m</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Holo Taco green mani</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hijf9usf3dwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1g9qrex</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>🗣️BRING 🗣️CRACKLE 🗣️NAIL 🗣️POLISH 🗣️BACK !!!!!!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9qrex</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1g9qq03</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite clear to black thermal </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9qq03/favorite_clear_to_black_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1g9qny6</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ephemeral Bluebird 🐦✨️ </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9qny6</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1g9qfim</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>The Perfect Blue for Fall</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9qfim</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1g9q9r1</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Orly bonder woes, and mixing with other base coats</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9q9r1/orly_bonder_woes_and_mixing_with_other_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1g9pyqf</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>🎃Jack O'Lanterns🎃</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9pyqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1g9pvns</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>How do i avoid getting laquer in my cuticles??? Polish: Cruel Mirage- Mooncat</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lh7ywr5rtcwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1g9pr1p</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Sticky base for regular nail polish</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9pr1p/sticky_base_for_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1g9pqis</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>What are my undertones??</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9pqis</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1g9plot</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Not sure how or why...</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoy5pvy2rcwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1g9p5fu</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Cirque Marsala Jelly matching my planner 🌺</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnqjb2qfocwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1g9ovj9</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>I am heartbroken</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvbntjofmcwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1g9ok0p</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>forces of evil ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9ok0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1g9oayt</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Seche Vive (gel) discoloration?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j35mvxeaicwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1g9nx2u</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>I've gotten SO many compliments out in the wild</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofs8vsfefcwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1g9nmax</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Holo Taco, One-Coat Black and Aurora Unicorn Skin 🦄</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hb6yu267dcwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1g9mz7e</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Clionadh - Hazard</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9mz7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1g9my8o</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Autumn leaves skittle mani</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9my8o/autumn_leaves_skittle_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1g9mia2</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ILNP and I am OBSESSED </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf2v0kc35cwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1g9lril</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Birefringence 🤩</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9lril</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1g9lm7y</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>First gel mani ✨</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am10sj6mybwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1g9lda8</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Nails Inc</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t4ih2gqwbwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1g9lb69</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Tried nail stickers for the first time and it’s so easy!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9lb69</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1g9lb3h</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a polish version of MAC's Blue Brown! </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9lb3h/looking_for_a_polish_version_of_macs_blue_brown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1g9l4x8</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alibi </t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9l4x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1g9kzy1</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Palate Cleanser</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i15es1rytbwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1g9kxo3</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Topcoat changing the color of the polish - What's going on here?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eis5s0jhtbwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1g9kej1</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Robin and Starfire nail art by andclaws. </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d3g5yuj7wqd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1g9k4vs</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Fairy dust as a topper on magnetics</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/erdg026knbwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1g9k1ts</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like it's giving traffic cone instead of pumpkin </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc6xoxnxmbwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1g9k0xv</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Boo!</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7hje46rmbwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1g9ge1x</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Pink sheer color suggestions?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9ge1x/pink_sheer_color_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1g9is8m</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>1st at home set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9is8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1g9if6b</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1eyzxz6abwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1g9i729</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>My try at artsy Halloween</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9i729</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1g9i5ir</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Halloween inspo</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9i5ir/halloween_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1g9h27t</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Chirality Factory Reset - gone forever/where to purchase? </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nne65eeeyawd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1g9gnio</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>OPIx Wicked Infinite Shine Ozmopolitan &amp; OPI’m Phosphorescent!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9gnio</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1g9g1r0</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Good nail polish companies in Germany?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g9g1r0/good_nail_polish_companies_in_germany/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1g9f9bk</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m going to call this new nail art trend ”baby woke up too soon from their nap” </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9f9bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1g9e04t</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Biodegradable nail polish</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://en.nano-sakura-shop.com/shop</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1g9zxd2</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Week 2 of Spooky Season </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9zxd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1g9ynvo</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I do like candy corn, mmm</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9ynvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1g9xpu6</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snake skin halloween press-ons set, hand painted </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6i14d3t9jewd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1g9wh8v</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Working on these and I really like how it’s coming along. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9wh8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1g9vfqg</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Baldur’s Gate 3 Nails! What should I make next?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9vfqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1g9ut8l</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">flash or superman?? </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fy3h65pudwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1g9u8tv</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I never thought that orange looked so good. </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuny45x9qdwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1g9tevg</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Spooky nails season by me.</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9tevg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1g9swn5</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So, you gotta boyfriend? </t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9swn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1g9sggb</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>I want to learn how to do my wife’s nails</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g9sggb/i_want_to_learn_how_to_do_my_wifes_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1g9r21l</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>My Agatha Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9r21l</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1g9qi23</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>halloween nails from my amazing nail tech!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9qi23</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1g9ohak</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Tamagotchi Press-on Nails by me</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9ohak</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1g9ln01</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>My nail inspo for Halloween. Let me see yours 👻</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn95vkgsybwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1g9k609</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>😽</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6m43m5tnbwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1g9ioou</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>hand painted halloween</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9ioou</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1g9hwu3</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Beginner Nail Art: pumpkinsss</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oyct2cw5bwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1g9hb9x</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Art the Clown from Terrifier</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1303cdyp0bwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1g9gdhl</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Ghibli nails by me. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9gdhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1g9e9gc</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Beginner - Rate my work please :)</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9e9gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1g9d1xv</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Does Anyone Else LOVE Big Gemstones/Charms?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g9d1xv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Oct 24 08:11:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_27.xlsx
+++ b/data/collected_data/2024_10_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C673"/>
+  <dimension ref="A1:C863"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11875,6 +11875,3236 @@
         </is>
       </c>
     </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1gaxf1q</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>a butterfly landed on me</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaxf1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1gaxer0</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>the nail i spent 5 months growing just broke.</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxpub8k4vnwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1gax3ea</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Like a perfect hair day, but for bare nails </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ovif9bmqnwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1gawphi</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>does tapered rectangle, or almond look best on my nails (or should i try another shape)?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gawphi</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1gawkte</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time ever doing press ons </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zonppbsijnwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1gaw1j9</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel x vs builder gel for nail growth </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdv5k3whcnwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1gavs77</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gavs77</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1gavfp9</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>First time got my nails done 🥰</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gavfp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1gag1s4</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Do these nails suit my hands?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klk3gjcxhjwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ganwow</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>E-File Advice Needed</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ganwow</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1gapssi</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>A little obsessed with my new fall cateye mani.</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gapssi</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1gauacn</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is my first time trying short almonds. What are your thoughts? </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6e8lgj2smwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1gau3gu</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gau3gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1gatuc7</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Can I buy only a specific nail tip size?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gatuc7/can_i_buy_only_a_specific_nail_tip_size/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1gatr89</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>One of my favorite gel x sets when I used to get them long 🥰</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13eu5ttlmmwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1gato7m</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Been into magnet looks lately</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brnnda3rlmwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1gatmxb</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Just a guy looking for a basic care routine</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gatmxb/just_a_guy_looking_for_a_basic_care_routine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1gatjt4</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Nails I’ve done this year for fun</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gatjt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1gati1f</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went for a deeper red </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gati1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1gasmja</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gelous Nail polishes 🙌🏼 </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kkndtgdbmwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1gasdf8</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gasdf8/is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1gas48n</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My nails for Halloween 🎃🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gas48n</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1garmzs</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got the perfect manicure today!! </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1garmzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1garf4i</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>First time fake nails</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1garf4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1gaqvc8</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Call me crazy but that’s ok lol </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gaqvc8/call_me_crazy_but_thats_ok_lol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1gaqnly</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>New Nails!!</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaqnly</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1gaqhqj</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Musings of a child </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaqhqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1gaq3dt</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Jelly Cay Eye Builder Gel</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fkih44zkolwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1gapnkg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Spooky nails I did for my sister…</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gapnkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1gaphyf</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>How did I do 😭</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8olefkcjlwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1gapdx4</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>I asked for Witchy Halloween nails</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gapdx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1gap6sn</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Anyone else who loves jewelry?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x88nfyfjglwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1gaogkx</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween 🎃 </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unnq4nwkalwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1gaog3a</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Pistachio gelato vibes</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gv1ytqfalwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1gaobjk</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Glow in the dark nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ud8rk18o9lwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1gaobmz</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>learning how to make custom press on nails :)</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag92eixo9lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1gao9o6</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Had all these plans to do vampy nail art but this color is too stunning 💅🏼</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gao9o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1ganz89</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i think i've finally found my perfect nude and perfect length!! </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv1j2nhn6lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1ganos0</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Hey there, just wanted to share my new manicure with a simple sweet dark metallic magenta!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuvr1pwe4lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1gano05</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>How to perfectly center charms/designs?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gano05/how_to_perfectly_center_charmsdesigns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1ganmkv</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Feeling spooky!!</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psn9y8ew3lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1ganc85</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>I believe they called it cat eye. Loving them!</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmqk3t6j1lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1ganadt</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Self portrait🤡😂</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ganadt</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1gan271</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gan271</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1gamt4q</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Halloween nails - black cat approved 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhfo7dy8xkwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1galneo</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Luxurious gel nails</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1galneo/luxurious_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1gamfpu</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>I'm in love with this simple combo</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gamfpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1galg96</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Which one do you prefer? Square or almond</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1galg96</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1galuf2</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Love this look!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu7lk0fspkwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1galg50</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Are these an additional $5 in length?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1galg50</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1galbeq</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Jelly Cay Eye Builder Gel</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a5on8uhtlkwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1gal5fo</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Dreamy vs. Vampire!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gal5fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1gaksk6</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>any critique? Ive been doing nails on myself for like 3 months noww idk if its good</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaksk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1gakhzb</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Bendy nails yah!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gakhzb/bendy_nails_yah/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1gake5e</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>I never worked so hard on a set in my life 🥹</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zc2srdxekwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1gak7tx</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Added ghosts (Thelma and Louise) to my nails because I'm not ready to part with this set yet</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9e7f3mmdkwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1gaju20</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>My spooky set!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o0975tisakwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1gajsuu</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>💜💚🧡 ILNP Halloween skittle 🎃💀 From thumb to pinky: Hallucinate, Flicker, Carved, Willow, Black Magic</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gajsuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1gajff5</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What type of nail application requires the least amount of drilling that damages cuticles? </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co6a9dps7kwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1gajf99</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I get my edges to stop lifting?? </t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh7enfdr7kwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1gajmlu</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>last year’s xmas nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gajmlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1gajfw7</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Spooky season, glitter nails!!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0jeowycv7kwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1gajes1</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Repair nailbeds</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gajes1/repair_nailbeds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1gajepv</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm looking for new nail ideas. I want something about fall 🍁🦊 2 or 3 nails different than others, but somehow special </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gajepv/im_looking_for_new_nail_ideas_i_want_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1gaj73h</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaj73h</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1gaj4f3</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>I returned to my style. I love them.!!!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0kcajch5kwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1gaj0p8</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Emily from corpse bride this year vs last year</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaj0p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1gaio0a</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>New nails who dis?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaio0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1gaifvu</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>does anyone else do their dominant hand short? is this weird?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jzlio2c0kwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1gai6fy</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>I ♡ maximalist sets</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jjogg2fxjwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1gai09r</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Would y’all pay for this set?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gai09r</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1gahy5j</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Spooky Babe👻</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gahy5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1gahk1z</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>how to fix crack in nails?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gahk1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1gagxhb</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Dnd gel sets</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gagxhb/dnd_gel_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1gagsqi</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Hello pumpkins and acorns</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gagsqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1gagh4c</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails! </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gagh4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1gagfug</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>₊✩‧₊˚౨ৎ˚₊✩‧₊</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49gfa0arkjwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1gageib</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Suggestions</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gageib</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1gag8q5</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Some press-ons I made for an event! How are they?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gag8q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1gaewmq</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>tips and tricks</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gaewmq/tips_and_tricks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1gaf05q</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Engagement shoot nails </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaf05q</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1gaezcv</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got my own dip nail kit the other day and gave it a try. Loved it! </t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7b3n5a6ajwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1gaeowk</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hen do nails. Theme was bright/festival </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8i8s3m18jwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1gaeoel</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Animal print nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaeoel</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1gaentd</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>What are alternative ways to open things?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gaentd/what_are_alternative_ways_to_open_things/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1gaeajx</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>How to remove shellac/gel?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gaeajx/how_to_remove_shellacgel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1gadxng</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>First time painting my nails. Scale 1 to 10, how bad are they?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qndt13l2jwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1gadtm2</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Red nail theory... but toes?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gadtm2/red_nail_theory_but_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1gaccgm</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Copper Nail Designs</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gaccgm/copper_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1ga7dz0</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time poster please be kind :) </t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga7dz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1ga7mbt</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Vacation Nails 🌺🌞</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga7mbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1gaa4t1</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>After acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaa4t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1gadk0m</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Fresh nails!!! 🖤🐆</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gadk0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1gadayd</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>my spooky szn set</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gadayd</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1gada4v</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>opinions?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx6trakpxiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1gad9b4</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍋 </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t9rg3pjxiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1gad4ui</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0ap3whmwiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1gad4g0</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Been doing clear gel to protect my nails after having gel x. This white stuff wasn’t there when I first put on my gel, it showed up overnight. Is it moisture?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srfwwn9iwiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1gad3vh</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I love it</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8gqn15fwiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1gad3di</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>She always kills it 😭</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7fe8ujbwiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1gax9j7</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>My Lurid Lacquer order came with four free polishes!!!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gax9j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1gavtt6</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Mulberry Fizzy</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r43v434t9nwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1gavmol</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Help With Mooncat?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gavmol/help_with_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1gavipn</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Nail art is my new favorite hobby</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gavipn</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1gav575</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>How do I ship nail polish?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gav575/how_do_i_ship_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1gasl3i</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Halloween Nails (might be a bit gross?)</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gasl3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1gasidu</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She’s back with another purple orange pairing </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gasidu</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1garz5q</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Halloween Sparkles</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1garz5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1garwbv</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Noodles Nail Polish- Hazy Harbors</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hi27lhyo4mwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1garqaz</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>SH Make Herstory</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1garqaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1gaq9nu</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The polish of my bog demon dreams </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaq9nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1gaq1gh</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>This moody fall rainbow from Glam Polish has me under it's spell 🔮✨ [gifted pr]</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=m8RhppQHCiY</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1gapmvs</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Tips for taking out Invisalign trays without breaking nails?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf8k86yjklwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1gapiix</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>🖤💚</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gapiix</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1gapfrq</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Why do you have to file off the colour when you want to get gel refilled?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gapfrq/why_do_you_have_to_file_off_the_colour_when_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1gaoz3z</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Queen of the Dead - Thermal </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaoz3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1gaoaa4</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>EdM Rise Again</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaoaa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1gao6z3</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Lots of Dots</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gao6z3</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1gao5d3</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>green chrome and clowns for the season</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gao5d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ganvhe</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Pumpkins</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qro89w206lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1gam7q0</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>❤️‍🩹❤️‍🩹❤️‍🩹</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gam7q0</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1gam036</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>“I don’t know.”</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghav3o90rkwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1gal5y2</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Can we talk about our tips to fight overconsumption and shopping our stash?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gal5y2/can_we_talk_about_our_tips_to_fight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1gal0jf</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>🎃 Halloweenie spoopy cats! 🎃</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gal0jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1gakmn2</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Haunted hues is so cool!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gakmn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1gakamv</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>LynB Halloween Advent Days 1-5 (Beetlejuice themed!)</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjgn8kwzdkwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1gajs0z</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>💜💚🧡 ILNP Halloween skittle 🎃💀 From thumb to pinky: Hallucinate, Flicker, Carved, Willow, Black Magic</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gajs0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1gajqpf</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Newbie Guy Needs Advice on Peeling Problem</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhw22mov9kwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1gaipki</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Wasn’t expecting to love the combo this much!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaiaqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1gai6mr</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>MENCHIE THE CAT</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cyldycfgxjwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1gahqnd</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Venom from ILNP</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bsjbhi5vtjwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1gahql2</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find this green Nail polish </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7381xbw5ujwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1gahnl7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Any indie holo/shimmer recommendations?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gahnl7/any_indie_holoshimmer_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1gahjrk</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Indomitable</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmyfkagtsjwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1gah5q9</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky Uranium Glass Nail Art </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gah5q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1gagq20</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>It’s ‘ween</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gagq20</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1gag9u5</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Quiet Corner </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9ew1umkjjwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1gag11m</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Help finding a nude?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gag11m</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1gaf97l</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Halloween Nails Activate</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ba0pf6i6cjwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1gaex8r</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>First time using a clean-up brush</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaex8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1gaeeun</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I may have a type</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaeeun</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1gae3o9</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>KB Shimmer Base Coats</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gae3o9/kb_shimmer_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1gae320</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This gradient makes me feel like a vampire </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gae320</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1gadvgz</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>twisted terracotta tanzanite 🥭</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaawev952jwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1gadpdc</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>[Ad] ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v06q6xav0jwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1gadiaa</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>😈😈</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gadiaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1gad0li</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn Nails </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gad0li</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1gaczan</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>A perfect example of a polish that is like a poor damsel indoors and a hot siren outdoors</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaczan</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1gacwl9</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Another vintage Rimmel!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gacwl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1gacvh6</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>salem ✨</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gacvh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1gact9y</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>ILNP Venom needs some love too! 🐍</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ags5lmm7uiwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1gacg2i</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>why do I love jelly nails on everyone else but hate it on myself 😭</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuv83lrhriwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1gabq08</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How often do you do a polish change? </t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gabq08/how_often_do_you_do_a_polish_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1gabogy</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>House of Hades is very pretty, I'm glad I have it, but I feel like it's not unique enough to justify the hype</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gabogy</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1gaa6i3</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I needed a screen break from my busy semester and put this together </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaa6i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1ga8yn0</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Top coat making nail polish soft underneath</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ga8yn0/top_coat_making_nail_polish_soft_underneath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1ga7pls</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Pastel spiderwebs for the Halloween season</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga7pls</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ga7hsm</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Can you develop a gel allergy on just one finger?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ga7hsm/can_you_develop_a_gel_allergy_on_just_one_finger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ga6dz6</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Nail polish pet peeves?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ga6dz6/nail_polish_pet_peeves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ga5ewx</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m going to a cat cafe later so I did my nails to match the occasion </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv5r1e52tgwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1gawgvq</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>4 hours of painting paid off😮‍💨</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8g9ou12inwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1gauoes</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Gothic Set</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8s5ykpbwmwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1gat283</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>ICP x TechN9 Nails 🫶🏻🤟🏼</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gat283</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1gaqyg2</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Vampire Nails 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaqyg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1gaqqtb</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>My graduation nails 🐸💚</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaqqtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1gapyut</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel x </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g7k3blbhnlwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1gapea9</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>My client’s NATURAL NAILS🤤</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/px9zk62gilwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1gap2tc</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Would you consider these nails to be short, or extra short? 💅</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw1dd9msflwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1gano4h</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Ready for the Halloween Party</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkh8bef94lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1gan8cc</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Starting to play around with charms and hand painted designs 🥰 #halloweennails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkwaczfn0lwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1gamwmq</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Pink and black spooky nails</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gamwmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1gam8ui</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Finally I got a new manicure after a couple of months of break. It was so difficult period of time! I still can’t used to the view of my short nails! How did I leave in past before gel polish?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqlsp6ovskwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1gakwlx</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Pretty Sets 🌺</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gakwlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1gakvl3</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Any critique plss ^^</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gakvl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1gakg9r</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I never work so hard on a nail set in my life 🥹</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a673sbvdfkwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1gak4bf</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Some nail art iv done in the past month and a half (:</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gak4bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1gajl2p</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>What color would look best under these cute little Halloween stickers?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ts8ox2w8kwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1gaixq6</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is my 1st attempt,be nice plz! </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaixq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1gais9l</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>🪐🪐🪐</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e3070grv2kwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1gai4tl</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>my HISS and brat summer nails</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gai4tl</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1gahl88</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Look like crystal ball </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gahl88</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1gahidt</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Fancy nails done by me</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akzu3j4jsjwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1gagvf9</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Hello pumpkins and acorns</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gagvf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1gagnxn</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>spooky set 👻💗</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gagnxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1gafdss</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Chucky and Tiffany!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9shh373djwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1gacjmj</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Louboutin nails </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwin9rg9siwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1gaa1uc</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>My set</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86683pwe8iwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ga8vrh</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>BDSM styled nails🥹</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q891ewiyxhwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ga8fg0</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Frank the Rabbit</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbr9l0fvthwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ga5ye0</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Which do you prefer?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ga5ye0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Oct 25 08:10:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_27.xlsx
+++ b/data/collected_data/2024_10_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C863"/>
+  <dimension ref="A1:C1062"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15105,6 +15105,3389 @@
         </is>
       </c>
     </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1gbnwei</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>did my nails for halloween! lmk how i did(:</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbnwei</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1gbnjr4</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Set I’m Making For Someone 💚</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rn2hcb78fuwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1gbnb0t</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Obsessed with my Halloween set</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngo6pakacuwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1gblv8d</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bloody Nails 🩸 My absolute favorite set like this yet. </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gblv8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1gbmk0x</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Scream themed nails</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbmk0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1gbmhij</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>A Starry Night set!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbmhij</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1gbmca5</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Anyone know where I can get this?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f269rce41uwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1gbkuwo</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>After 1.5 years of simple nails, I’m back on the fancy train!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbkuwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1gbku6u</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blo*d splatter  nail design </t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbku6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1gbkngf</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One Glowy Bat a** nail! </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s0xoqcmjtwd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1gbkltv</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>New black &amp; white Nails🖤🤍</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g95egzb6jtwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1gbkfx2</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Cat eyes!! Thanks girls</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbkfx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1gbk4cf</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Halloween nails 🍁💅</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sog8n6eetwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1gbk0ws</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haloween nails 💅 what other colour combo should i use ? </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/milk7hlidtwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1gbjuxf</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2nxl0cvbtwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1gbjtnm</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>are these good? im still a beginner so pls be nice ✨🙏</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmib9yaibtwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1gbjq3i</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I love this cat press-on nails! so cute</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbjq3i/i_love_this_cat_presson_nails_so_cute/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1gbjl6i</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Day 5 with OPI xPRESS/On nails and I’m feeling like I might never got back to the salon ✨</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asjgbdp89twd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1gbjhqf</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Back to my roots w French..kept the toes red tho 🤣</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rorakqac8twd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1gbjchp</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>I got my nails doneeee 🤧❤️✨</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbjchp</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1gbj3og</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>What’s the white mark on my nail?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80wjdyxk4twd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1gbilr1</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbilr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1gbihuj</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Set 🎃 👻 </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbihuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1gbiabe</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Do square nails look good on me?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xduphatuwswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1gbia2e</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>ready for halloween ?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbia2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1gbap7z</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Making press ons - how to know gel is cured?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbap7z/making_press_ons_how_to_know_gel_is_cured/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1gbgdik</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Nail injury - recovery process</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbgdik/nail_injury_recovery_process/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1gbgxor</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absolutely new to nails: what do I ask for? </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbgxor/absolutely_new_to_nails_what_do_i_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1gbhm4d</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Vampire Vibes 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgrg10llqswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1gbh4sz</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Queen of Hearts</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hpiz9yamswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1gbgng7</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does square look good on me? </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xgwcuj1iswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1gbg4qf</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Fall festive nails</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpgyeryldswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1gbgeid</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing my own Gelx full set. Not perfect, but not trash. </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbgeid</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1gbg945</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quite Literally Dead Inside </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2l139scmeswd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1gbfxte</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>First timer</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui6hjcvzbswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1gbffbo</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urb8p9jn7swd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1gbfc19</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>When you're a pinky pink girl and also love halloween 👻🩷</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9xh45qv6swd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1gbekyg</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Fran bow nails!!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5nyk9ds0swd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1gbekdl</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>My nail girl never disappoints 💅</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15jjpg4o0swd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1gb9rjt</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can a salon fix this without going full acrylic? </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iada54fvzqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1gbdypf</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Spooky Season 🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sl53psopvrwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1gbdnf5</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All of my favorite recent nails! </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdnf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1gbdmmm</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>I worked so hard :(</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdmmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1gbdjtk</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Finally my long nails are back</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdjtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1gbdinm</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Anyone know why my pinky nails are angling upwards?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdinm</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1gbdgn1</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Not loving my nails now 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g8wpucsrrwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1gbd5o0</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Simple Halloween nails 🎃</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbd5o0</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1gbd3q9</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> New Cat Eye set 💫</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wtoc0390prwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1gbc6ym</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favourite colour so far </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ejguh43irwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1gbbrd5</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Best glue for fake nails?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdqc37averwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1gbahkt</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>How much time do my babies have left</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn83pya85rwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1gbacxo</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>My Halloween nails</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbacxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1gba1st</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I thought these bb’s looked good shining in the morning light </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhqcomhz1rwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1gb9yyl</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb9yyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1gb9xv0</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>My newest set feat. Edgar Allan Poe 🖤</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb9xv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1gb9qxc</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>god I love my top coat!!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gtmr6tqzqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1gb95jn</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone knows if you can use melodysusie cordless pen drills with a cord? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb95jn/does_anyone_knows_if_you_can_use_melodysusie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1gb8scw</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Fall Nails 💅🍂</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiemau8osqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1gb8oph</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>In love with my cateyes!!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb8oph</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1gb8kh8</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>How to paint my wonky nail</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytdrnx4xqqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1gb8b0e</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Vampire</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb8b0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1gb7nwp</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7nwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1gb7ldh</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Coraline set I did!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7ldh</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1gb7iz5</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>nail dreams coming true 🖤</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr4j5vq8jqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1gb7ij9</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Square -&gt; Oval</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7ij9</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1gb7h1t</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Radioactive nails for the spooky season</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7h1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1gb7fzo</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Belated Nail Set</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp5i37zliqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1gb7cxj</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set = a whole new woman </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mio7m6zhqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1gb6k6u</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Electric buffer or nail file suggestions?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb6k6u/electric_buffer_or_nail_file_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1gb66uz</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Spooky Nails</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/atl3eqg79qwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1gb642v</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Manicure for Halloween, I really love these things</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi82w99p8qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1gb60gt</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know how to fix this? </t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb60gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1gautl4</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Press on amateur 💙</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gautl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1gb15ip</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DO NOT BUY THE JODSONE GEL KIT FROM AMAZON!! </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb15ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1gb5z5h</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>This Hello Kitty press-on set is everything! I’m obsessed🩷</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6dcd1oo7qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1gb3p85</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there a way to salvage these? </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb3p85</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1gb3wns</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>How to tell my tech my gel nails didn’t cure correctly?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb3wns/how_to_tell_my_tech_my_gel_nails_didnt_cure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1gb5h7f</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Should I continue getting my nails done?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t44rd3dy3qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1gb5pka</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Natural nails newbie advice</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb5pka/natural_nails_newbie_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1gb5psv</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>What shape/length nails for bony, delicate , arthritic hands ?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb5psv/what_shapelength_nails_for_bony_delicate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1gb5py7</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Halloween nails 👀🩸🎃💀 tried to do a green chrome over nude but it doesn’t really show 😂</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb5py7</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1gb5er6</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love the colour so much that had to do my toes </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb5er6</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1gb5dlv</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do we think </t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfm9pc673qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1gb54en</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Ok my turn...</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbxj8z3b1qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1gb4tjs</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Anniversary nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb4tjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1gb3sap</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Third time trying to do my own nails, finally decent result! (Gel x)</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb3sap</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1gb3bz1</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun colours for Spring/Summer 💜🩷🩵 </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzx9liqinpwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1gb2ncb</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Nail newb who got gel extensions too long and can barely type. Flight today — what services do I need to shorten/repaint and how long do they take? </t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb2ncb</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1gb2ark</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to prevent nail polish fast chipping? </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb2ark/how_to_prevent_nail_polish_fast_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1gb1z04</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Cute Halloween / Spooky Themed Nails</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb1z04</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1gb1aql</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>short pink nails</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3p8dnpk5pwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1gb1587</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>AAHH!!! Real Monster nails! OC</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb1587</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1gb0y6w</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Sort of short</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48am57v52pwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1gaz83b</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Press on win!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grxfafbrjowd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1gb0812</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Topcoat wars! </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gb0812/topcoat_wars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1gb0562</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g500ziw8uowd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1gayn9p</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growing journey with gels at home! </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gayn9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1gayjwf</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let my manicurist choose 😌 </t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7ezfym7bowd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1gaxplm</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>How much is your nail care expense per month?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gaxplm/how_much_is_your_nail_care_expense_per_month/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1gaxm5x</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>July &gt; Now</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukm1fxa5ynwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1gbnya5</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for October PPU Great Balls of Ice? </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n3pr8zjkuwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1gbni72</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Indies Without Balls?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbni72/indies_without_balls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1gbl2pl</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Similar color? </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25jevf3qntwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1gbk6gr</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new fav?? </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbk6gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1gbk1q5</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Bought some polish at Cosme in Japan and wanted to swatch.</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbk1q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1gbjvni</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Spooky</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbjvni</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1gbjtdx</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Quick and simple-ish Halloween</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbjtdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1gbjm70</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Nails I did very quickly for my Oscar the Grouch costume today</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbjm70</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1gbjbwm</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Essie Hard to Resist Glow &amp; Shine and China Glaze Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnbsboqs6twd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1gbiket</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Witch's ball, my beloved</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qarlmd0izswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1gbhh80</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Water based top coat?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbhh80/water_based_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1gbgpwu</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My comfort polish 😻 OPI Show us your tips! </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbgpwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1gbgfp0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>First Night Owl Lacquer</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbgfp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1gbg7gj</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>After three costs on all nails, the full thing is 5ml, is this a good amount to use ot is it too much?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbg7gj</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1gbfcv1</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Your favorite blurring base coat?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbfcv1/your_favorite_blurring_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1gbf5al</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little shimmery, velvety, spoopy splatter </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbf5al</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1gbf0q8</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>A spooky shimmery skittle</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbf0q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1gbetb4</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Jior Couture - Highly Flammable Sept 24 PPU</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/six60dlf2swd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1gbem1g</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer- My Favorite Spooky B*tch</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsb6v8vt0swd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1gbdsky</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat, if you read this, please make a whole toppers collection </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdsky</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1gbdpgh</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I call him Rob</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8a9gqbiotrwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1gbdmvy</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Similar to My bugs my bugs </t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10uimhq4trwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1gbdcoz</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Why do I always have to potty RIGHT after I paint my nails??</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdcoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1gbd4cd</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>First attempt with stamping plates</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tcvu1ov4prwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1gbcun2</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pictures can't capture how pretty this is. </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxb6fq3lmrwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1gbcix9</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Whatever You Do, Don't Fall Asleep</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbcix9</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1gbbaen</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Glinda the Good </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbbaen</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1gbb57z</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Opal mani for my birthday 💖</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0f8sbs67arwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1gbawl4</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Just want to share this red for autumn 🍁</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbawl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1gbaqtv</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The swap/sell subreddit. </t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbaqtv/the_swapsell_subreddit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1gbaom1</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Exceptional wear</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0o3b3pp6rwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1gbana8</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Which brands have the most unique or exciting polishes to you?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbana8/which_brands_have_the_most_unique_or_exciting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1gbafl0</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>🦇Minty Spoopy Cute🦇</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbafl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1gba8wp</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>For those who love light sheers, what are your favorite pink sheer nail polishes?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gba8wp/for_those_who_love_light_sheers_what_are_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1gba0sz</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>My GITD Halloween Birthday Nails 🎃🎉</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gba0sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1gb98vu</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Holiday Anti-consumerism</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gb98vu/holiday_anticonsumerism/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1gb968t</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone knows if you can use melodysusie cordless pen drills with a cord? </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gb968t/does_anyone_knows_if_you_can_use_melodysusie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1gb910i</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's fall am I right?! </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb910i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1gb8p5s</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Quite literally dead insporkle</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb8p5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1gb89zx</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>It’s a (Halloween) Party on My Nails!</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6ejesktoqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1gb8076</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Opening the LynB Beetlejuice advent polishes…part 1!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb8076</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1gb7r4b</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Cock-a-doodle Doom!!</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7r4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1gb7n4x</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wonderland by Patty Lopes </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7n4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1gb7m5i</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>My first ever attempt at builder gel</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7302dnvjqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1gb7gyw</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>New to nail art, here are some of my recent attempts</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb7gyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1gb7bpt</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>The Stakes Are Deadly - Dan Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctzm5j5qhqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1gb74w0</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Re-rack! All ORLY in one place (finally!)</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbugpgpagqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1gb6kx8</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>bday ILNP haul!!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb6kx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1gb6f5d</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Mooncat - Sealed with a Hiss</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hq6y4bxxaqwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1gb6b9n</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where can I find this beauty or something similar? Photo found on Pinterest </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9erkrrd5aqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1gb6am3</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Keep or redo?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb6am3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1gb66cf</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>First stamping attempt</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb66cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1gb658j</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>My attempt at Moo Deng nails 🦛💅🏼</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2bhtlow8qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1gb61tz</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Sin Eater + Fallen Flakie Taco!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gs02eus78qwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1gb5yxd</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Fixed my disappointing treachery in the blue by wearing it over hot pink polish!</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1ac10um7qwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1gb547l</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>First attempt at nail art for fall</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1k815j781qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1gb4vcn</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Mulled Wine</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb4vcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1gb4c4q</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forced into the Nub Club </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb4c4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1gb3mqv</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bright &amp; Spooky! The perfect color for these last warm days of October. </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb3mqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1gb3k1d</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Comfy sweater and cute ghost nails 👻</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb3k1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1gb3hsz</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Mooncat</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gb3hsz/mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1gb3c1b</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Rogue Laquers “Let’s get dangerous” 💟</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb3c1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1gb3b46</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>I made my first nail polish and it actually turned out okay</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h8xcf4dnpwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1gb34e4</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Joined the Indomitable club 💜</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21ny43pslpwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1gb32tv</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Fall forward</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb32tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1gb2r3h</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Cuticula CHOCOLAATE! With Nuts</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb2r3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1gaauy6</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>what are some things i can use to support my broken, gel damaged nails while i hopefully grow them out, is dip powder or builder gel an option or do i need the missing parts to regrow first (the picture is after gel x removal and i am a habitual nail biter and nail picker)</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gaauy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1gaqsfv</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Any good hypoallergenic gel brand recs?</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gaqsfv/any_good_hypoallergenic_gel_brand_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1gaydj6</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Help me find this colour</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/figyfjgv8owd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1gaytmv</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails always distract me at work. The velvet effect has worn off, but I’m still obsessed with the subtle red shift. </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aaoea2jteowd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1gayhu8</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>No horseshoe magnet velvet nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pploohhaowd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1gaxwc8</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Can regular Sally Hanson nail polish cause contact dermatitis? I have been applying it on my skin for years.</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gaxwc8/can_regular_sally_hanson_nail_polish_cause/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1gbox0x</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Finished my Halloween set 🎃</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbox0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1gbn1jc</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Halloween!!! But different 😏</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbn1jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1gbm97f</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Scream set for Halloween</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbm97f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1gblvtk</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Absolute favorite set of bloody nails yet 🩸🤌🏼</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gblvtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1gbkzee</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Junji Ito set!!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbkzee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1gbkn7c</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">siren nails for halloween </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbkn7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1gbi9og</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Nails for Aftershock Concert</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbi9og</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1gbhezo</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really enjoyed doing these nails! </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbhezo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1gbgz76</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>The 2nd set I’ve done! Love doing nail art so far</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk757juwkswd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1gbfu8x</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice, Beetlejuice,Beetlejuice! </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbfu8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1gbe9sm</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>skeleton set for spooky month</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbe9sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1gbdcnw</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>My first set 3D</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbdcnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1gb9poy</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Heat Signature Nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pjindb7hzqwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1gb9513</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone knows if you can use melodysusie cordless pen drills with a cord? </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gb9513/does_anyone_knows_if_you_can_use_melodysusie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1gb70gj</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My jobs yesterday ! </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnsrmm2efqwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1gb66tf</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>These bautys</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ieggql79qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1gb62jv</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More nails </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwwogh6e8qwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1gb5qw4</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Halloween nails 👀🩸🎃💀 tried to do a green chrome over nude but it doesn’t really show 😂</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb5qw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1gb4hwl</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>My first three gel sets :)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb4hwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1gb2v57</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today’s vibe ✌🏻 glistening darkness </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/411dh5smjpwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1gb2mha</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After my post inquiring about the color yesterday, I couldn’t decide so I did 1 nude and 1 dark red. </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb2mha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1gb2it4</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb2it4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1gb2688</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween set!!!! </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb2688</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1gb254r</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No stickers everything hand drawn .. first time doing this </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb254r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1gb1yby</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Cute Halloween / Spooky Themed Nails</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gb1yby</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1gb1t7m</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>This gel design makes my hands look less thin</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tqu21xgapwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1gacmw5</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Pumpkin patch</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8lcjxyxsiwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Oct 26 08:09:25 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_27.xlsx
+++ b/data/collected_data/2024_10_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1062"/>
+  <dimension ref="A1:C1254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18488,6 +18488,3270 @@
         </is>
       </c>
     </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1gcg5l5</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">are these too thick? </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okj5xkhq52xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1gcfw7o</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>The Official Halloween Set 🎃</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcfw7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1gcfsbt</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Finally grew my nails out to a length I’m happy with and celebrated with tortoise shell!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90hfvwxl02xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1gcfsbo</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I got yesterday </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvnqirrl02xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1gcfplx</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Basic press ons</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcfplx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1gcfk0r</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>red jelly on me by me :)</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru14wyzcx1xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1gcf7qm</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Wasn’t going to post these, but I switched from acrylic to gel.</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txajj60ss1xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1gcdyq7</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>New Custom Press On Set!! Inspired by Death Valley NP!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcdyq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1gcc8lg</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Finally did those Pinterest fall nails 🍂🍁✨</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcc8lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1gc95n1</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>halloween nails 🕸❤️</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwwa0il6yzwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1gc5jab</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>She’s bloody vicious 🤭🩸</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc5jab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1gc3v10</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>New set. Inspired by a post here yesterday!</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pku0jp30pywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1gc240s</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Essie Wicked gel dupe??</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gc240s/essie_wicked_gel_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1gc23tu</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Gel nail polish color looks different on my nails vs the color the bottle says</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gc23tu/gel_nail_polish_color_looks_different_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1gcedfh</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jumping into the Chrome trend with some DIY press-ons </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2g7wf4xh1xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1gcec16</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>First attempt application</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcec16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1gcea8i</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Love💙</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f59uvg2sg1xd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1gce327</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tryin’ ombre nails </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gce327</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1gcdula</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Halloween French Tips</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcdula</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1gcdeem</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Which shape is best for me?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcdeem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1gcd5we</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>how much should i tip?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alzfqc5k31xd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1gccyxu</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>How bad do these look??</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gccyxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1gccu2m</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry cola nails 🍒 </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwhmjdq001xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1gccqs3</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Nails without UV/Curing or Acrylic?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gccqs3/nails_without_uvcuring_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1gcca69</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>would gel cure through these?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcca69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1gcbsre</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY'd some press ons, not sure how I feel about them </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okfw6txvo0xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1gcb6hx</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Wedding Nails!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcb6hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1gcauv9</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Halloween Ideas?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcauv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1gcall6</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>My daughter does her own nails</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcall6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1gca7yt</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Favorite Beginner Nail Art</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gca7yt/favorite_beginner_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1gca6u4</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>After a month of rest, I made this set for my best friend. I really loved the result. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkbovjy680xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1gca3je</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>I should have done more bling</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lfc8q1b70xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1gca1pn</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry Shortcake🍰🍓 </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6eyrhaq60xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1gca10v</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Getting a manicure and set of nails for first time tomorrow</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5v2u31k60xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1gc9t8p</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Went dark and rounded for the first time ever… still adjusting.</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc9t8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1gc9hjm</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Showing my spooky season cat my spooky season nails </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mp4s3qc10xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1gc9806</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Nightmare before Christmas</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc9806</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1gc96ex</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape suits me best </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc96ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1gc93ui</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Spooky Ghosts</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8ltxfppxzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1gc8zym</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little splatter for Halloween </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm8wldaqwzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1gc8vzw</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Tips for press on nails?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hglhmhpvzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1gc8kku</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>I got a new nail set from my nail tech yay!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgnidfzqszwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1gc8gel</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails on myself! </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaedzfforzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1gc8ep5</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$90 Russian manicure in LCOL city-fading after 2 days? Is this normal? V beauty pure Rose Quarts base and gel topcoat. Appointment total before tip was $120. I use rubber gloves when cleaning </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc8ep5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1gc8db7</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Claws </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cyrbywxqzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1gc82we</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc82we</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1gc7trb</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Set </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch8c82t1mzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1gc7nrb</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>First try!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc7nrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1gc7fr8</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>i love my nail tech DOWN</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gnp59tlizwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1gc78s8</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">witchy celestial nails </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qshykbxgzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1gc6q4k</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Going in a concert date &amp; chose to get his favorite color. I tried something new &amp; instead of a straight line French, I got a wavy line.</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hcr8jeeczwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1gc6min</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Clowns for Halloween 🤡</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc6min</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1gc6k33</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Anyone know where to pick up a good clear cateye gel topper polish?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gc6k33/anyone_know_where_to_pick_up_a_good_clear_cateye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1gc6bde</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Purple for Halloween 🔮</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t0c1sl8z8zwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1gc64qi</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mom's nails for her first U of O football game. </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ctpf3xe7zwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1gc61ap</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Happy SpOoKy season 🎃</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y96nq7nj6zwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1gc611d</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>🎃</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/233bbegk6zwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1gc547l</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Refill?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfvrqki3zywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1gc4r1t</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>just wanted to show my favorite set so far i’ve done…</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc4r1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1gc4pjr</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Such a simple yet elegant design</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5jcrhxsvywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1gc4j6v</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need opinions! What shape suits my hand better? </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc4j6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1gc4a97</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">are these bad pls be honest </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ditjv9tbsywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1gc3xnw</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My mom’s nails!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc3xnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1gc3rq2</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and white </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc3rq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1gc33y1</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>basic nails</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ci2zjh8jywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1gc2uvh</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>This is so so pretty OMG I’m obsessed. I don’t even wanna wear them. Someone take me to a ball 😍</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pv6em0b9hywd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1gc2qo6</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Loving this blue 😇</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ho34hlegywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1gc2hjl</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>What colors would go well with my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lf7lxrwdeywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1gc2e1z</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>New nail sets 🥰</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc2e1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1gc1m3r</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>advice needed 🙈</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc1m3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1gc1eov</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Tried doing some halloween nail art on my natural nails instead of extentions for once!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc1eov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1gc13y1</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark sparkles for Halloween </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc13y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1gc11nk</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Amber cat eye gel set 😍 Obsessed is an understatement</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xlhqq153ywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1gc0io1</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Pearly nudes</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isq6yuq3zxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1gc0glr</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Bent my nail</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5abtxakoyxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1gc0d8s</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>First time gel nail extensions!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfq0heoyxxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1gc01rk</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Peanut Butter Jelly Nails!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc01rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1gc01ec</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Nail Reformation</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epva1e0gvxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1gc00jw</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Biab fans, is this normal?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc00jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1gbzxln</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little glam for an all black outfit. </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbzxln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1gbzxl7</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Need black dark nail polish recs !!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbzxl7/need_black_dark_nail_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1gbzvy9</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Cotton candy/marshmallow nails</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib204al9uxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1gbvlx7</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>feeling witchy!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbvlx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1gbnajz</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Really worried salon used MMA on me….</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbnajz/really_worried_salon_used_mma_on_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1gbpb05</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Acrylic pain?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbpb05</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1gbzehr</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>This Is Some Boo Sheet</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dp7jv99iqxwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1gbuq0y</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Black elegant french tips 🖤</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pviugjfgqwwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1gbmzvr</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Orly repair kit - questions!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbmzvr/orly_repair_kit_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1gbz476</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>tigress set 🐅🧡</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbz476</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1gbyydu</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Accidentally used nail glue as debonder on my press on nails. What should I do?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbyydu/accidentally_used_nail_glue_as_debonder_on_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1gby3cz</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">info on design? </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5tzt4jkgxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1gbxcha</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>cousin did my bday nails ♥️ (@gabysnailz)</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8in8i0zaxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1gbx9dg</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Embarrassing but…</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbx9dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1gbwx4c</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my 2024 nail journey hehe </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbwx4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1gbwp7f</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Matte polish durability?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gbwp7f/matte_polish_durability/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1gbwoq3</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Nails too chunky? Wedding nails</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbwoq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1gbwmck</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>i think they came out freaking cute since i’m a beginner right?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbwmck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1gbwiha</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Fav set I did in a while💅🏼</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfw4b7jj4xwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1gbvu62</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Abstract silver lines</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb4hxo1fzwwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1gbv5te</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Ombré Fall Nails 🍂</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6idm5ft0uwwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1gcfv6b</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>First set of gel x nails</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qlepyuq12xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1gcfuxk</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Can't decide what colour to do for the week, suggestions?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ayn267i12xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1gcem79</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I finally bought a glass nail file and I understand the hype now</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gcem79/i_finally_bought_a_glass_nail_file_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1gcdjxp</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Seeking recs for black polish with green undertones?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gcdjxp/seeking_recs_for_black_polish_with_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1gccc7l</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do my nails bend like that? </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a0tqoikru0xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1gcaxua</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Freshly assembled battlestation</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/46yl8uowf0xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1gcak3q</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>How do you prevent vertical cracks from forming on your polish?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gcak3q/how_do_you_prevent_vertical_cracks_from_forming/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1gcac5b</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Oops, matched my drink.</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcac5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1gca372</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Please recommend a dupe? Fancy gloss Evergreen</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz3ebq4370xd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1gc9y1z</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Holo Taco dupes?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc9y1z/holo_taco_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1gc9pda</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Thermals with bright, contrasting color combos?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc9pda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1gc96g0</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive and June Gel - can you still get an allergic reaction to it? </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc96g0/olive_and_june_gel_can_you_still_get_an_allergic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1gc8xzo</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mooncat ROOT OF ALL EVIL </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc8xzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1gc8lxg</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>I don't normally wear a single polish on my left hand, but when I do it's a flakie BOMB</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc8lxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1gc7rmr</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bottle’s last coat. It was a good run and I’m sad to say goodbye to her. </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc7rmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1gc71vl</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>FYI: Fancy Gloss store is now  open</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc71vl/fyi_fancy_gloss_store_is_now_open/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1gc70sj</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wolf Spider Surprise </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x7wizvqhezwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1gc6tbm</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>A bit darker than Essie Sugar Daddy</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc6tbm/a_bit_darker_than_essie_sugar_daddy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1gc6gv4</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Monsters Inc. Nails: Adorable Closet Doors &amp; Mischievous Monsters! 👾👹</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc6gv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1gc5ve0</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Glow-in-the-dark Ghosts</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc5ve0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1gc587p</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">accidentally matched with my blanket </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc587p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1gc55i5</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Third Try at French Tips (Newbie Still)</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc55i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1gc55fo</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>quick “bloody” nails for a halloween party tomorrow!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc55fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1gc4wls</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>I know this is a longshot...</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc4wls/i_know_this_is_a_longshot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1gc4p2u</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Forbidden fruit</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kplv1w7pvywd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1gc4np9</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slowly growing out efile damage </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ut69bmjevywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1gc4jd0</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Essie Ballet Slippers</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc4jd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1gc49fw</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>ILNP Hidden Paths for fall</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc49fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1gc36ix</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Clionadh Psilocybin 😪🍄🤩🤯</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e6jbf0mrjywd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1gc2zvj</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Fall skittle 🍁</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc2zvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1gc2v9q</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glowy Halloween nails! </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc2v9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1gc2uvb</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>B&amp;W matte glitter toppers?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc2uvb/bw_matte_glitter_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1gc27ux</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Need black dark nail polish recs !!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gc27ux/need_black_dark_nail_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1gc1ijm</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this count as prugly? </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0oshciju6ywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1gc1fej</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>The Rainbow Fish by me</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vgp0lui56ywd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1gc12ui</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Halloween Party Ready!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc12ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1gc0w85</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Zoya + ILNP</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc0w85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1gc0vou</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>I’ve been wondering what this design reminded me of and I finally got it</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/614ywy1u1ywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1gc0hye</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Pearly nudes</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7di725ryyxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1gbzz5a</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goblins and Ghoulies! </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbzz5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1gbzw5c</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Covering nail stains </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbzw5c/covering_nail_stains/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1gbzp6x</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>I just got back into doing my nails and I love this color!</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbzp6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1gbzp0e</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>“Is it red or purple?”  “Yes”</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mqgz1nrsxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1gbzjb2</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Atomic Polish hosts polish making workshops. I made this :).</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i96kes99rxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1gbz75s</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is some boo sheet </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/72j7oq5woxwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1gbyvbh</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>My favorite manicure that I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbyvbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1gbyrvo</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to match my Halloween dress </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbyrvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1gbyrah</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Base Coat </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhf0iw5ilxwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1gbylm4</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>psycho</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbylm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1gbyi7l</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>PFD Prehalloween</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbyi7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1gbycif</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>my take on a Halloween colour scheme</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbycif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1gbya2n</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Radioactive blue</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbya2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1gby4pn</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Finally got around to trying out Holo Taco and I'm in love ✨</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/709kihctgxwd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1gbxl4k</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried to do a little Halloween themed combo. Not sure how I feel about it. </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbxl4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1gbwxee</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I present to you... ✨Gradient à la nail dust✨</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ehi4zkq7xwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1gbufii</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question About Recent Manicure Experience </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gbufii/question_about_recent_manicure_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1gbu6al</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Victorian Varnish issues</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbu6al</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1gbswgf</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Vampire vs Werewolf</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbswgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1gbs38a</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>ILNP Amber (cateye) / unedited photos</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbs38a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1gbqxsj</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Halloweeny nails 💅🏻🔪🩸</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbqxsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1gbqhv4</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Cirque - Folie à deux</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbqhv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1gbq7to</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>(Previous paid pr) Potion Perfect from 7 Mystery Boos and Porcelain from Colores De Carol for another Halloween mani ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbq7to</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1gcfxrb</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>First set of gel x extensions</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vigzkm2q22xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1gcee8l</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Just finished a set of nails for my friend</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbguesd7i1xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1gcebnu</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>This reminds me of scarecrow stitches</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1262v3p9h1xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1gbwvls</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Couldn’t decide on Halloween design, so I stuck with flowers..</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1q8psvc7xwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1gce1cw</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>New Custom Press On Set Inspired by Death Valley NP!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gce1cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1gcdj8z</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Made a chaotic Halloween set for my sister</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcdj8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1gcdgnh</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Super super proud of this set!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/klgzchts61xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1gcc679</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Silver Freestyle set. What your think? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcc679</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1gcavh3</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>My First Set of Gels.</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x94xo39f0xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1gcanoy</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>My daughter does her own nails</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wuotrg20d0xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1gcafiv</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>All eyes are on my nails this Halloween! By @kalsrebelliousnails on IG</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcafiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1gc92k8</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Handmade </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h334e7tdxzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1gc88a7</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i love my nail tech &lt;3 @ktnails.251 on insta </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joxow5vnpzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1gc5tx6</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blood splatter spooky nails </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc5tx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1gc4ubx</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3D sculpting nail design, happy to see my skill improved </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r8p1uzt9wywd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1gc4o3r</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Such a simple yet elegant design</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg73jzphvywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1gc3vlr</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Halloween prepping 🎃</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o2yf0t6pywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1gc32l7</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Halloween nail art</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgiqyn1yiywd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1gc2byw</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>New nail sets 💕</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc2byw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1gc1rkl</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Halloween Manicure </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc1rkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1gbx3sh</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? Any good glue you recommend for these press ons? </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh3uzh049xwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1gbwk7n</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Think my daughter loves Spider man 🕷️🤣</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz3vse3x4xwd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1gbwebt</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another Halloween set to match my pirate costume! Loved how these turned out! </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbwebt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1gbwc0j</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>How do you guys do the black splatter on that white nail? I want it so bad but my nail tech can't seem to do it.. or know how to</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmvkf7c53xwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1gbv3ti</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Credits to me, love how i did this set</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbv3ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1gbu802</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails! </t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70a244z4mwwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1gbteif</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dr Frank-n-Furter </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbteif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1gbsxpa</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Bloody nails for the remainder of October 🩸🩸</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfo7r3ipawwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1gbs38t</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Pumpkin Jack</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gbs38t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1gbrnta</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to share my newest nails here </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7se1h0bxvwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Oct 27 08:10:31 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_27.xlsx
+++ b/data/collected_data/2024_10_27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1254"/>
+  <dimension ref="A1:C1414"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21752,6 +21752,2726 @@
         </is>
       </c>
     </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1gd5ug0</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>tips for taking photos for nails</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg8jqnhj79xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1gd5e3n</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>First manicure after getting back into nail art – I had forgotten how much I love doing my nails</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gd5e3n/first_manicure_after_getting_back_into_nail_art_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1gd5huu</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>First time using black polish 🖤🩶🖤🤍🎃</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd5huu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1gd4tts</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time doing gelX, how cooked am I? </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd4tts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1gd4pvu</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Halloween Nails!! Any improvements?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5shsy2vbs8xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1gd4k35</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Fun Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd4k35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1gd4duq</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vi2mv32o8xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1gd43gf</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>if my nails can fly, i can too</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gd43gf/if_my_nails_can_fly_i_can_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1gd38xo</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>I did my girlfriend’s nails! First time doing someone else’s nails!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vylg6ou0a8xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1gd3e42</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>French!</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lue3t80lb8xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1gd2j37</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Happy Halloween 👻</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd9bk1p028xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1gd2gql</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails done in Tokyo :) </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q68rwshc18xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1gd2diz</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Pokemon Blues</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd2diz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1gd1qtz</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd1qtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1gd1ozn</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Ready for fall! 🍁</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oseoo3j0t7xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1gd1cqc</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Black matte for the fall</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd1cqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1gd1as1</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Finally!</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dpeadpdvo7xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1gd0mm0</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My spooky Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cg2ucjoog7xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1gczx2f</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Love my nails</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gczx2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1gczpx1</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can't beat a classic red nail! (and some springtime mandarin picking) </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gczpx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1gczkii</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Feeling ~blue~</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jogx2jbs67xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1gczc6p</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Advice Needed - Handmade Press-Ons Pealing?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gczc6p/advice_needed_handmade_pressons_pealing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1gcy82c</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Subtle Spooky Mani</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcy82c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1gcy62b</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Is there some kind of frenzy for magnetic nail polish</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gcy62b/is_there_some_kind_of_frenzy_for_magnetic_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1gcxved</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat disaster </t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcxved</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1gcxqsp</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>my first rubber base gel mani! any suggestions? :)</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87cma9zjp6xd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1gcxmnw</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>It’s so hard type with long nails and trying to pick up spilt coins is nearly impossible</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jflr7swio6xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1gcxc29</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>NAILZZZZZ DID</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcxc29</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1gcwydf</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Not too bad for 'press ons'</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcwydf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1gcwivw</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>experimenting with blooming gel today</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26i7o7mte6xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1gcu5d2</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>growing out bitten nails</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gcu5d2/growing_out_bitten_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1gcvd8e</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Tried out new set of stickers 🍁🍂✨</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcvd8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1gcuqw2</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>My SHEIN special 🫶</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tcfjhmoz5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1gcupvm</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>DIY Halloween nails 🧛🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcupvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1gcu6la</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Growing out my nails again - which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcu6la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1gcsyne</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>October set</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbr65m0mk5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1gctron</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>I’ve bitten my nails my whole life.</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gctron</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1gctbc4</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31c9wrmmn5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1gct8eu</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t go wrong with classic red for autumn </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gct8eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1gct670</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Happy Halloween</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gct670</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1gcsw4m</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My first time trying gel nails. What do we think?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcsw4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1gcsm4r</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Feeling like a Pink Glitter Disco Ball 🪩</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rp809dqlh5xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1gcsftn</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Press on cheapies…..</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnorwsx7g5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1gcserv</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>chrome butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zd8d3mwyf5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1gcs5dj</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Got my first Nail extensions &amp; I'm loving it ! 💅🏻🫡🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nc19ic3wd5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1gcs44m</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails in Korea </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b27pw03md5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1gcrt24</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Still thinking about my nails from last year🖤</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuec63r2b5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1gcrnwu</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>💜💕🩶</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6z3fksw95xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1gcrj9c</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Newbie to manicures color recommend for a better skin tone match?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcrj9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1gcre2h</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>New Nail Shape, Who Dis?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a11e89zm75xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1gcr5sx</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8iqp3is55xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1gcr4co</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New GelX set </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcr4co</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1gcr3xh</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Halloween Set </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcr3xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1gcqsca</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Square or almond?</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcqsca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1gcqs5m</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yv3hywq25xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1gcqs4h</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Frosty for fall</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4edbllq25xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1gcqlkx</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been obsessed with cute clown nails lately so I had to give them a try. </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcqlkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1gcqf6o</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cadillacquer - I Would Die For You </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcqf6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1gcqey8</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Cat eye with chrome</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhru9v1pz4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1gcqakh</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lisa Frank Halloween 👻 </t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7bzrflqy4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1gcq6wn</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>got my nails done in china</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcq6wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1gcptve</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Any idea why everytime I get my nails done the right hand index finger always feel uncomfortable?</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gcptve/any_idea_why_everytime_i_get_my_nails_done_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1gcp2sn</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Bruising from lifting/bending or something else?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t2tftivo4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1gco487</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Press-ons to match my glitter kitty pants😻</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5ryzqz4h4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1gciwl2</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Does anyone know how to use these products?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gciwl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1gcooor</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Mommy/daughter Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcooor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1gcol83</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my tattoo artist gets nails, i get a tattoo :) </t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2at2bzuk4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1gcoir6</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>What do y’all rate it out of 10 (design,length, shape)</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcoir6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1gcofm5</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>I little vamp but also cute 😀</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcofm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1gco3cw</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>DIY Tortoise Shell Gel X!</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emfs0ryxg4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1gcnzqp</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to share my recently done nails! </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcnzqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1gcn8k6</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Manicure bubbling after shower??</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcn8k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1gcmeeu</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Paint the autumn pink🍂</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcmeeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1gcmafb</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>My halloween set</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65gb07r424xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1gcm5g0</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Recreation design by u/Anxoous_Lobster_8069 with glow in the dark</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcm5g0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1gcm3s8</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The prettiest nails I’ve ever had </t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uuzkouki04xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1gclwpo</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Halloween nails: not perfect, but they make me happy 👻</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gyk2yhuy3xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1gclofs</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Did nails on my mom, how did I do?</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vk56tg7uw3xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1gcku19</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first set! </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcku19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1gckfw9</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Multiple different nail designs for three events over two days of wedding</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gckfw9/multiple_different_nail_designs_for_three_events/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1gck74b</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried </t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcyk7932j3xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1gchc2p</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Previous set for my birthday / holiday to Greece 🇬🇷 </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x219icetl2xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1gchbwa</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Can I change the paint of my gel nails?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gchbwa/can_i_change_the_paint_of_my_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1gchaqz</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had my nails done Thursday ☺️ wanted something autumn vibes </t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m74phibbl2xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1gch3q5</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gch3q5/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1gcgptx</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Does this look bad?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsk1rlpfd2xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1gcfy7b</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Beginner baby over here. Gluing help for acrylics ?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gcfy7b/beginner_baby_over_here_gluing_help_for_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1gcg2gx</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is about my 10th DIY set using builder - I love them but struggling with shapes/curing and finding lumps </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcg2gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1gd57io</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Magnetic help please?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gd57io/magnetic_help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1gd4jpk</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>sassy sauce polish omg!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd4jpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1gd3np0</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas polishes with red &amp; green flakies? </t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gd3np0/christmas_polishes_with_red_green_flakies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1gd215b</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Atomic Sherbert by ILNP topped with Black Flakie Taco by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tw5wgtcmw7xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1gd14it</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Reign by ILNP to Match the Rain</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd14it</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1gd0tgk</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Spiced Cider</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn48zseqj7xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1gd06yb</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gd06yb/great_lakes_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1gd06ok</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Holo Taco - Peridon’t Bother Me</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd06ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1gczrw8</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Does anyone know how I can prevent this from happening?</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjbynpht87xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1gczoep</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Evil Dead nails</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gczoep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1gczleg</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Cock-a-doodle Doom is Moira Rose Approved</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gczleg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1gczg0t</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Cirque Colors Delusions of Grandeur chromed</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k1tk9cph57xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1gcylu2</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Halloween blood mani</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcylu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1gcycjs</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>A PPU delivery? On MY birthday?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcycjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1gcy47u</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Well I HAD Halloween nails 🥲</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocspavc0t6xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1gcxx7s</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Y'ALL</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcxx7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1gcxru3</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Growth Update </t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcxru3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1gcxlz2</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Facebook shorts and "the gap"</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gcxlz2/facebook_shorts_and_the_gap/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1gcwu4v</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Halloween nails ready</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcwu4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1gcw7jy</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Supporting cast for a walrus costume</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcw7jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1gcvsss</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A couple of Fall/Halloween-ish manis </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcvsss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1gcvo0j</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Misbehaving </t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcvo0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1gcvib3</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer's Fading Light</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ovgbb6m066xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1gcvcfi</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Ohhh myyyy</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0bgvjfyr46xd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1gcutcy</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Thermal blood drip mani 💉🩸</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcutcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1gctrdy</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Halloween nails (with bonus cat 🐈‍⬛)</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j49wygl3r5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1gct5k3</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Real world pics of Phoenix Watermelon Tourmaline?</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scssrod9m5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1gct1qw</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Pink and black to match my Halloween costume!</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gct1qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1gcszzx</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>A dupe for the wet n wild fergie  polish?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kupqwdxk5xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1gcrjip</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>💜💕🩶</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfq0bvhw85xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1gcqvr5</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>"Eternal Glow" is right. 10 minute mani</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcqvr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1gcqfa6</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>💚💛🧡❤️🤎</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcqfa6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1gcqdt2</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cadillacquer - I Would Die For You </t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcqdt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1gcqc6a</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Do Rainbow Connection do a Black Friday sale?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gcqc6a/do_rainbow_connection_do_a_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1gcpq05</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyp-nautical from Sally Hansen miracle gel is so GORGEOUS!! </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcpq05</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1gcpcwc</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Blood splatter nails for Halloween!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcpcwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1gcp3z2</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Poison Apple Nails 🍎</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcp3z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1gcow5a</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails done! </t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bscv2jcn4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1gcomwt</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“No nail polish” nail polish nails </t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcomwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1gco8bl</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Fall Vibes but Make it Spooky</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gco8bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1gco378</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lurid Lacquer has me in a chokehold </t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gco378</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1gcny9t</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>I Need Vampy Shimmery Polish Recs 🖤🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4t6kgpssf4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1gcnduq</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love loud nails </t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcnduq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1gcmujw</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Not exhaustive, but an excellent source to track polish name, release, and collection information if you're interested in that sort of thing</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.lacquertracker.com/browse</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1gcmcsf</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Unexpected Visitor</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv0schxo24xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1gcm8p2</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Autumn colors and some fancy.</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4f64uwp14xd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1gcl2ce</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Efile Accident</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gcl2ce/efile_accident/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1gckv4c</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Colores de Carol - Pumpkin Head (Sept ‘24 PPU)</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gckv4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1gck80h</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Hooked!! All the combo possibilities!</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gck80h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1gcjz3h</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Having fun with some designs</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcjz3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1gcjlg8</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Who ya gonna call? 🎶🎶</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcjlg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1gc4icn</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>ILNP Enchantment (with &amp; without flash)</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gc4icn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1gc7jxr</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails!! </t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssrll3cmjzwd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1gcfpoz</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for the perfect 80s pink </t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eycx8mflz1xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1gci75i</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>2024 Polish Advent Calendars</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gci75i/2024_polish_advent_calendars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1gci3nf</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Possibly my favourite polish ever!</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gci3nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1gchnkd</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Scorpio has a chokehold on me</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gchnkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1gchc0t</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>if looks could kill ✨💀</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gchc0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1gd1l2f</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some art I’ve (43m) done for my daughter (12f) lately. </t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd1l2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1gd1czw</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Was feeling creepy👀</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gd1czw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1gcyacy</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>had to get one more silly set from my tech @/_jennathecreator_ !!</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcyacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1gcxuo3</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Did some Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwlv5e5lq6xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1gcw0dq</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>First time using blooming gel for this kinda design. I'm happy with it</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh1jookha6xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1gcvg9p</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>vivienne westwood nails</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcvg9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1gcr5fk</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Happy Halloween from my yearly set of bloody tips!</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gn4kahp55xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1gcpakh</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tortious Shell for Autumn </t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msb3fcplq4xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1gcn2e9</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Christmas wrapping green and gold!</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcn2e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1gcm23o</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Recreation design by u/Anxious_Lobster_8069 with glow in dark</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcm23o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1gck2q6</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Cat eye autumn nails</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bd8cqpuuh3xd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1gcjvns</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Non-UV cure rhinestone glue?</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gcjvns/nonuv_cure_rhinestone_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1gcingl</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat nails for my daughter 💕 </t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj2o2zhd23xd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1gcgzgu</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Autumn nails by me</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gcgzgu</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>